<commit_message>
Updates to the Burndown chart prior to our Sprint 3 review
</commit_message>
<xml_diff>
--- a/Sprints/Sprint-Backlog-Burndown-Chart.xlsx
+++ b/Sprints/Sprint-Backlog-Burndown-Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conwaycmoravian.edu/Courses/234/sandwichTruckProj./Sprints/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abatotmoravian.edu/MyCourses/234/sandwichTruckProj./Sprints/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7638BB6B-D29B-5F48-855D-8385693FD479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657A5658-0577-4144-907D-2959AFAFF290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog #2" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="63">
   <si>
     <t>User Story #1</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Task: Modifying Routes</t>
+  </si>
+  <si>
+    <t>Task: Add sandwich ordrs to the list</t>
   </si>
 </sst>
 </file>
@@ -549,28 +552,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>48</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1588,9 +1591,9 @@
   </sheetPr>
   <dimension ref="B1:AC126"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1825,22 +1828,22 @@
         <v>8</v>
       </c>
       <c r="H6" s="9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I6" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J6" s="9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K6" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L6" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M6" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1881,16 +1884,16 @@
         <v>1</v>
       </c>
       <c r="J7" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -1931,16 +1934,16 @@
         <v>4</v>
       </c>
       <c r="J8" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K8" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L8" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M8" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -2156,7 +2159,7 @@
         <v>4</v>
       </c>
       <c r="M13" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -2316,7 +2319,7 @@
         <v>3</v>
       </c>
       <c r="K17" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="9">
         <v>0</v>
@@ -2448,14 +2451,30 @@
         <v>40</v>
       </c>
       <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
+      <c r="F21" s="9">
+        <v>10</v>
+      </c>
+      <c r="G21" s="9">
+        <v>9</v>
+      </c>
+      <c r="H21" s="9">
+        <v>5</v>
+      </c>
+      <c r="I21" s="9">
+        <v>5</v>
+      </c>
+      <c r="J21" s="9">
+        <v>5</v>
+      </c>
+      <c r="K21" s="9">
+        <v>2</v>
+      </c>
+      <c r="L21" s="9">
+        <v>1</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0</v>
+      </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
@@ -2475,19 +2494,37 @@
     </row>
     <row r="22" spans="2:29" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="9" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
+      <c r="F22" s="9">
+        <v>2</v>
+      </c>
+      <c r="G22" s="9">
+        <v>2</v>
+      </c>
+      <c r="H22" s="9">
+        <v>2</v>
+      </c>
+      <c r="I22" s="9">
+        <v>2</v>
+      </c>
+      <c r="J22" s="9">
+        <v>2</v>
+      </c>
+      <c r="K22" s="9">
+        <v>2</v>
+      </c>
+      <c r="L22" s="9">
+        <v>0</v>
+      </c>
+      <c r="M22" s="9">
+        <v>0</v>
+      </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -2740,35 +2777,35 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5">
         <f>SUM(F5:F29)</f>
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="G30" s="5">
         <f>SUM(G6:G29)</f>
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="H30" s="5">
         <f t="shared" ref="H30:M30" si="0">SUM(H5:H29)</f>
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I30" s="5">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="J30" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="L30" s="5">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="M30" s="5">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>

</xml_diff>